<commit_message>
siguen fallando los prompts
</commit_message>
<xml_diff>
--- a/script_master_data/ficherosExcelOrigen/DED-AceleracionBacklog_Adopcion IA_v2a.xlsx
+++ b/script_master_data/ficherosExcelOrigen/DED-AceleracionBacklog_Adopcion IA_v2a.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\6003305\Documents\tarea\estimacionIA_jdk21\script_master_data_beltran\ficherosExcelOrigen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\6003305\Documents\tarea\estimacionIA_jdk21\script_master_data\ficherosExcelOrigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E8E47A-7ED3-4F0A-8EA2-50CCF444AC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEACAEA-7A2C-4B92-BCEE-CC6C8530997F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdopcionIA" sheetId="1" r:id="rId1"/>
@@ -3021,6 +3021,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="B1:BR178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -8744,7 +8745,7 @@
         <v>N</v>
       </c>
     </row>
-    <row r="82" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="9"/>
       <c r="C82" s="147"/>
       <c r="D82" s="10"/>
@@ -8789,7 +8790,7 @@
       <c r="AQ82" s="28"/>
       <c r="AR82" s="28"/>
     </row>
-    <row r="83" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="9"/>
       <c r="C83" s="147"/>
       <c r="D83" s="10"/>
@@ -8834,7 +8835,7 @@
       <c r="AQ83" s="28"/>
       <c r="AR83" s="28"/>
     </row>
-    <row r="84" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="9"/>
       <c r="C84" s="147"/>
       <c r="D84" s="10"/>
@@ -8879,7 +8880,7 @@
       <c r="AQ84" s="28"/>
       <c r="AR84" s="28"/>
     </row>
-    <row r="85" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="9"/>
       <c r="C85" s="147"/>
       <c r="D85" s="10"/>
@@ -8924,7 +8925,7 @@
       <c r="AQ85" s="28"/>
       <c r="AR85" s="28"/>
     </row>
-    <row r="86" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="9"/>
       <c r="C86" s="147"/>
       <c r="D86" s="10"/>
@@ -8969,7 +8970,7 @@
       <c r="AQ86" s="28"/>
       <c r="AR86" s="28"/>
     </row>
-    <row r="87" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="9"/>
       <c r="C87" s="147"/>
       <c r="D87" s="10"/>
@@ -9014,7 +9015,7 @@
       <c r="AQ87" s="28"/>
       <c r="AR87" s="28"/>
     </row>
-    <row r="88" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="9"/>
       <c r="C88" s="147"/>
       <c r="D88" s="10"/>
@@ -9059,7 +9060,7 @@
       <c r="AQ88" s="28"/>
       <c r="AR88" s="28"/>
     </row>
-    <row r="89" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="9"/>
       <c r="C89" s="147"/>
       <c r="D89" s="10"/>
@@ -9104,7 +9105,7 @@
       <c r="AQ89" s="28"/>
       <c r="AR89" s="28"/>
     </row>
-    <row r="90" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="9"/>
       <c r="C90" s="147"/>
       <c r="D90" s="10"/>
@@ -9149,7 +9150,7 @@
       <c r="AQ90" s="28"/>
       <c r="AR90" s="28"/>
     </row>
-    <row r="91" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="9"/>
       <c r="C91" s="147"/>
       <c r="D91" s="10"/>
@@ -9194,7 +9195,7 @@
       <c r="AQ91" s="28"/>
       <c r="AR91" s="28"/>
     </row>
-    <row r="92" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="9"/>
       <c r="C92" s="147"/>
       <c r="D92" s="10"/>
@@ -9239,7 +9240,7 @@
       <c r="AQ92" s="28"/>
       <c r="AR92" s="28"/>
     </row>
-    <row r="93" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="9"/>
       <c r="C93" s="147"/>
       <c r="D93" s="10"/>
@@ -9284,7 +9285,7 @@
       <c r="AQ93" s="28"/>
       <c r="AR93" s="28"/>
     </row>
-    <row r="94" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="9"/>
       <c r="C94" s="147"/>
       <c r="D94" s="10"/>
@@ -9329,7 +9330,7 @@
       <c r="AQ94" s="28"/>
       <c r="AR94" s="28"/>
     </row>
-    <row r="95" spans="2:44" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:44" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="9"/>
       <c r="C95" s="147"/>
       <c r="D95" s="10"/>
@@ -9373,7 +9374,7 @@
       <c r="AQ95" s="28"/>
       <c r="AR95" s="28"/>
     </row>
-    <row r="96" spans="2:44" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:44" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B96" s="9"/>
       <c r="C96" s="147"/>
       <c r="D96" s="10"/>
@@ -9418,7 +9419,7 @@
       <c r="AQ96" s="28"/>
       <c r="AR96" s="28"/>
     </row>
-    <row r="97" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="9"/>
       <c r="C97" s="147"/>
       <c r="D97" s="10"/>
@@ -9463,7 +9464,7 @@
       <c r="AQ97" s="28"/>
       <c r="AR97" s="28"/>
     </row>
-    <row r="98" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="9"/>
       <c r="C98" s="147"/>
       <c r="D98" s="10"/>
@@ -9508,7 +9509,7 @@
       <c r="AQ98" s="28"/>
       <c r="AR98" s="28"/>
     </row>
-    <row r="99" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="9"/>
       <c r="C99" s="147"/>
       <c r="D99" s="10"/>
@@ -9553,7 +9554,7 @@
       <c r="AQ99" s="28"/>
       <c r="AR99" s="28"/>
     </row>
-    <row r="100" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="9"/>
       <c r="C100" s="147"/>
       <c r="D100" s="10"/>
@@ -9598,7 +9599,7 @@
       <c r="AQ100" s="28"/>
       <c r="AR100" s="28"/>
     </row>
-    <row r="101" spans="2:44" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:44" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="9"/>
       <c r="C101" s="147"/>
       <c r="D101" s="10"/>
@@ -9643,7 +9644,7 @@
       <c r="AQ101" s="28"/>
       <c r="AR101" s="28"/>
     </row>
-    <row r="102" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="9"/>
       <c r="C102" s="147"/>
       <c r="D102" s="10"/>
@@ -9688,7 +9689,7 @@
       <c r="AQ102" s="28"/>
       <c r="AR102" s="28"/>
     </row>
-    <row r="103" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="9"/>
       <c r="C103" s="147"/>
       <c r="D103" s="10"/>
@@ -9733,7 +9734,7 @@
       <c r="AQ103" s="28"/>
       <c r="AR103" s="28"/>
     </row>
-    <row r="104" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="9"/>
       <c r="C104" s="147"/>
       <c r="D104" s="10"/>
@@ -9778,7 +9779,7 @@
       <c r="AQ104" s="28"/>
       <c r="AR104" s="28"/>
     </row>
-    <row r="105" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="9"/>
       <c r="C105" s="147"/>
       <c r="D105" s="10"/>
@@ -9823,7 +9824,7 @@
       <c r="AQ105" s="28"/>
       <c r="AR105" s="28"/>
     </row>
-    <row r="106" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="9"/>
       <c r="C106" s="147"/>
       <c r="D106" s="10"/>
@@ -9868,7 +9869,7 @@
       <c r="AQ106" s="28"/>
       <c r="AR106" s="28"/>
     </row>
-    <row r="107" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="9"/>
       <c r="C107" s="147"/>
       <c r="D107" s="10"/>
@@ -9913,7 +9914,7 @@
       <c r="AQ107" s="28"/>
       <c r="AR107" s="28"/>
     </row>
-    <row r="108" spans="2:44" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:44" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="9"/>
       <c r="C108" s="147"/>
       <c r="D108" s="10"/>
@@ -9958,7 +9959,7 @@
       <c r="AQ108" s="28"/>
       <c r="AR108" s="28"/>
     </row>
-    <row r="109" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="9"/>
       <c r="C109" s="147"/>
       <c r="D109" s="10"/>
@@ -10003,7 +10004,7 @@
       <c r="AQ109" s="28"/>
       <c r="AR109" s="28"/>
     </row>
-    <row r="110" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="9"/>
       <c r="C110" s="147"/>
       <c r="D110" s="10"/>
@@ -10048,7 +10049,7 @@
       <c r="AQ110" s="28"/>
       <c r="AR110" s="28"/>
     </row>
-    <row r="111" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="9"/>
       <c r="C111" s="147"/>
       <c r="D111" s="10"/>
@@ -10093,7 +10094,7 @@
       <c r="AQ111" s="28"/>
       <c r="AR111" s="28"/>
     </row>
-    <row r="112" spans="2:44" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:44" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="9"/>
       <c r="C112" s="147"/>
       <c r="D112" s="10"/>
@@ -10138,7 +10139,7 @@
       <c r="AQ112" s="28"/>
       <c r="AR112" s="28"/>
     </row>
-    <row r="113" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B113" s="9"/>
       <c r="C113" s="147"/>
       <c r="D113" s="10"/>
@@ -10183,7 +10184,7 @@
       <c r="AQ113" s="28"/>
       <c r="AR113" s="28"/>
     </row>
-    <row r="114" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="9"/>
       <c r="C114" s="147"/>
       <c r="D114" s="10"/>
@@ -10228,7 +10229,7 @@
       <c r="AQ114" s="28"/>
       <c r="AR114" s="28"/>
     </row>
-    <row r="115" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="9"/>
       <c r="C115" s="147"/>
       <c r="D115" s="10"/>
@@ -10273,7 +10274,7 @@
       <c r="AQ115" s="28"/>
       <c r="AR115" s="28"/>
     </row>
-    <row r="116" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B116" s="9"/>
       <c r="C116" s="147"/>
       <c r="D116" s="10"/>
@@ -10318,7 +10319,7 @@
       <c r="AQ116" s="28"/>
       <c r="AR116" s="28"/>
     </row>
-    <row r="117" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="9"/>
       <c r="C117" s="147"/>
       <c r="D117" s="10"/>
@@ -10363,7 +10364,7 @@
       <c r="AQ117" s="28"/>
       <c r="AR117" s="28"/>
     </row>
-    <row r="118" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="9"/>
       <c r="C118" s="147"/>
       <c r="D118" s="10"/>
@@ -10408,7 +10409,7 @@
       <c r="AQ118" s="28"/>
       <c r="AR118" s="28"/>
     </row>
-    <row r="119" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="9"/>
       <c r="C119" s="147"/>
       <c r="D119" s="10"/>
@@ -10453,7 +10454,7 @@
       <c r="AQ119" s="28"/>
       <c r="AR119" s="28"/>
     </row>
-    <row r="120" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="9"/>
       <c r="C120" s="147"/>
       <c r="D120" s="10"/>
@@ -10498,7 +10499,7 @@
       <c r="AQ120" s="28"/>
       <c r="AR120" s="28"/>
     </row>
-    <row r="121" spans="2:70" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:70" ht="42.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="9"/>
       <c r="C121" s="147"/>
       <c r="D121" s="10"/>
@@ -10543,7 +10544,7 @@
       <c r="AQ121" s="28"/>
       <c r="AR121" s="28"/>
     </row>
-    <row r="122" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B122" s="9"/>
       <c r="C122" s="147"/>
       <c r="D122" s="10"/>
@@ -10588,7 +10589,7 @@
       <c r="AQ122" s="28"/>
       <c r="AR122" s="28"/>
     </row>
-    <row r="123" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="9"/>
       <c r="C123" s="147"/>
       <c r="D123" s="10"/>
@@ -10659,7 +10660,7 @@
       <c r="BQ123" s="106"/>
       <c r="BR123" s="106"/>
     </row>
-    <row r="124" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B124" s="9"/>
       <c r="C124" s="147"/>
       <c r="D124" s="10"/>
@@ -10704,7 +10705,7 @@
       <c r="AQ124" s="28"/>
       <c r="AR124" s="28"/>
     </row>
-    <row r="125" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B125" s="9"/>
       <c r="C125" s="147"/>
       <c r="D125" s="10"/>
@@ -10749,7 +10750,7 @@
       <c r="AQ125" s="28"/>
       <c r="AR125" s="28"/>
     </row>
-    <row r="126" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="9"/>
       <c r="C126" s="147"/>
       <c r="D126" s="10"/>
@@ -10794,7 +10795,7 @@
       <c r="AQ126" s="28"/>
       <c r="AR126" s="28"/>
     </row>
-    <row r="127" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="9"/>
       <c r="C127" s="147"/>
       <c r="D127" s="10"/>
@@ -10839,7 +10840,7 @@
       <c r="AQ127" s="28"/>
       <c r="AR127" s="28"/>
     </row>
-    <row r="128" spans="2:70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:70" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B128" s="9"/>
       <c r="C128" s="147"/>
       <c r="D128" s="10"/>
@@ -10884,7 +10885,7 @@
       <c r="AQ128" s="28"/>
       <c r="AR128" s="28"/>
     </row>
-    <row r="129" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B129" s="9"/>
       <c r="C129" s="147"/>
       <c r="D129" s="10"/>
@@ -10929,7 +10930,7 @@
       <c r="AQ129" s="28"/>
       <c r="AR129" s="28"/>
     </row>
-    <row r="130" spans="2:44" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:44" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="9"/>
       <c r="C130" s="147"/>
       <c r="D130" s="10"/>
@@ -10974,7 +10975,7 @@
       <c r="AQ130" s="28"/>
       <c r="AR130" s="28"/>
     </row>
-    <row r="131" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B131" s="9"/>
       <c r="C131" s="147"/>
       <c r="D131" s="10"/>
@@ -11019,7 +11020,7 @@
       <c r="AQ131" s="28"/>
       <c r="AR131" s="28"/>
     </row>
-    <row r="132" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B132" s="9"/>
       <c r="C132" s="147"/>
       <c r="D132" s="10"/>
@@ -11064,7 +11065,7 @@
       <c r="AQ132" s="28"/>
       <c r="AR132" s="28"/>
     </row>
-    <row r="133" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="9"/>
       <c r="C133" s="147"/>
       <c r="D133" s="10"/>
@@ -11109,7 +11110,7 @@
       <c r="AQ133" s="28"/>
       <c r="AR133" s="28"/>
     </row>
-    <row r="134" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="9"/>
       <c r="C134" s="147"/>
       <c r="D134" s="10"/>
@@ -11154,7 +11155,7 @@
       <c r="AQ134" s="28"/>
       <c r="AR134" s="28"/>
     </row>
-    <row r="135" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B135" s="9"/>
       <c r="C135" s="147"/>
       <c r="D135" s="10"/>
@@ -11199,7 +11200,7 @@
       <c r="AQ135" s="28"/>
       <c r="AR135" s="28"/>
     </row>
-    <row r="136" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B136" s="9"/>
       <c r="C136" s="147"/>
       <c r="D136" s="10"/>
@@ -11244,7 +11245,7 @@
       <c r="AQ136" s="28"/>
       <c r="AR136" s="28"/>
     </row>
-    <row r="137" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B137" s="9"/>
       <c r="C137" s="147"/>
       <c r="D137" s="10"/>
@@ -11289,7 +11290,7 @@
       <c r="AQ137" s="28"/>
       <c r="AR137" s="28"/>
     </row>
-    <row r="138" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B138" s="9"/>
       <c r="C138" s="147"/>
       <c r="D138" s="10"/>
@@ -11334,7 +11335,7 @@
       <c r="AQ138" s="28"/>
       <c r="AR138" s="28"/>
     </row>
-    <row r="139" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B139" s="9"/>
       <c r="C139" s="147"/>
       <c r="D139" s="10"/>
@@ -11379,7 +11380,7 @@
       <c r="AQ139" s="28"/>
       <c r="AR139" s="28"/>
     </row>
-    <row r="140" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="9"/>
       <c r="C140" s="147"/>
       <c r="D140" s="10"/>
@@ -11424,7 +11425,7 @@
       <c r="AQ140" s="28"/>
       <c r="AR140" s="28"/>
     </row>
-    <row r="141" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B141" s="9"/>
       <c r="C141" s="147"/>
       <c r="D141" s="10"/>
@@ -11469,7 +11470,7 @@
       <c r="AQ141" s="28"/>
       <c r="AR141" s="28"/>
     </row>
-    <row r="142" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B142" s="9"/>
       <c r="C142" s="147"/>
       <c r="D142" s="10"/>
@@ -11514,7 +11515,7 @@
       <c r="AQ142" s="28"/>
       <c r="AR142" s="28"/>
     </row>
-    <row r="143" spans="2:44" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:44" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B143" s="9"/>
       <c r="C143" s="147"/>
       <c r="D143" s="10"/>
@@ -11559,7 +11560,7 @@
       <c r="AQ143" s="28"/>
       <c r="AR143" s="28"/>
     </row>
-    <row r="144" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B144" s="9"/>
       <c r="C144" s="147"/>
       <c r="D144" s="10"/>
@@ -11604,7 +11605,7 @@
       <c r="AQ144" s="28"/>
       <c r="AR144" s="28"/>
     </row>
-    <row r="145" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B145" s="9"/>
       <c r="C145" s="147"/>
       <c r="D145" s="10"/>
@@ -11649,7 +11650,7 @@
       <c r="AQ145" s="28"/>
       <c r="AR145" s="28"/>
     </row>
-    <row r="146" spans="2:44" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:44" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B146" s="9"/>
       <c r="C146" s="147"/>
       <c r="D146" s="10"/>
@@ -11694,7 +11695,7 @@
       <c r="AQ146" s="28"/>
       <c r="AR146" s="28"/>
     </row>
-    <row r="147" spans="2:44" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:44" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B147" s="9"/>
       <c r="C147" s="147"/>
       <c r="D147" s="10"/>
@@ -11739,7 +11740,7 @@
       <c r="AQ147" s="28"/>
       <c r="AR147" s="28"/>
     </row>
-    <row r="148" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B148" s="9"/>
       <c r="C148" s="147"/>
       <c r="D148" s="10"/>
@@ -11784,7 +11785,7 @@
       <c r="AQ148" s="28"/>
       <c r="AR148" s="28"/>
     </row>
-    <row r="149" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B149" s="9"/>
       <c r="C149" s="147"/>
       <c r="D149" s="10"/>
@@ -11829,7 +11830,7 @@
       <c r="AQ149" s="28"/>
       <c r="AR149" s="28"/>
     </row>
-    <row r="150" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B150" s="9"/>
       <c r="C150" s="147"/>
       <c r="D150" s="10"/>
@@ -11874,7 +11875,7 @@
       <c r="AQ150" s="28"/>
       <c r="AR150" s="28"/>
     </row>
-    <row r="151" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B151" s="9"/>
       <c r="C151" s="147"/>
       <c r="D151" s="10"/>
@@ -11919,7 +11920,7 @@
       <c r="AQ151" s="28"/>
       <c r="AR151" s="28"/>
     </row>
-    <row r="152" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B152" s="9"/>
       <c r="C152" s="147"/>
       <c r="D152" s="10"/>
@@ -11964,7 +11965,7 @@
       <c r="AQ152" s="28"/>
       <c r="AR152" s="28"/>
     </row>
-    <row r="153" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B153" s="9"/>
       <c r="C153" s="147"/>
       <c r="D153" s="10"/>
@@ -12009,7 +12010,7 @@
       <c r="AQ153" s="28"/>
       <c r="AR153" s="28"/>
     </row>
-    <row r="154" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="9"/>
       <c r="C154" s="147"/>
       <c r="D154" s="10"/>
@@ -12054,7 +12055,7 @@
       <c r="AQ154" s="28"/>
       <c r="AR154" s="28"/>
     </row>
-    <row r="155" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B155" s="9"/>
       <c r="C155" s="147"/>
       <c r="D155" s="10"/>
@@ -12099,7 +12100,7 @@
       <c r="AQ155" s="28"/>
       <c r="AR155" s="28"/>
     </row>
-    <row r="156" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B156" s="9"/>
       <c r="C156" s="147"/>
       <c r="D156" s="10"/>
@@ -12144,7 +12145,7 @@
       <c r="AQ156" s="28"/>
       <c r="AR156" s="28"/>
     </row>
-    <row r="157" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B157" s="9"/>
       <c r="C157" s="147"/>
       <c r="D157" s="10"/>
@@ -12189,7 +12190,7 @@
       <c r="AQ157" s="28"/>
       <c r="AR157" s="28"/>
     </row>
-    <row r="158" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B158" s="9"/>
       <c r="C158" s="147"/>
       <c r="D158" s="10"/>
@@ -12234,7 +12235,7 @@
       <c r="AQ158" s="28"/>
       <c r="AR158" s="28"/>
     </row>
-    <row r="159" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B159" s="9"/>
       <c r="C159" s="147"/>
       <c r="D159" s="10"/>
@@ -12279,7 +12280,7 @@
       <c r="AQ159" s="28"/>
       <c r="AR159" s="28"/>
     </row>
-    <row r="160" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B160" s="9"/>
       <c r="C160" s="147"/>
       <c r="D160" s="10"/>
@@ -12324,7 +12325,7 @@
       <c r="AQ160" s="28"/>
       <c r="AR160" s="28"/>
     </row>
-    <row r="161" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B161" s="9"/>
       <c r="C161" s="147"/>
       <c r="D161" s="10"/>
@@ -12369,7 +12370,7 @@
       <c r="AQ161" s="28"/>
       <c r="AR161" s="28"/>
     </row>
-    <row r="162" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B162" s="9"/>
       <c r="C162" s="147"/>
       <c r="D162" s="10"/>
@@ -12414,7 +12415,7 @@
       <c r="AQ162" s="28"/>
       <c r="AR162" s="28"/>
     </row>
-    <row r="163" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B163" s="9"/>
       <c r="C163" s="147"/>
       <c r="D163" s="10"/>
@@ -12459,7 +12460,7 @@
       <c r="AQ163" s="28"/>
       <c r="AR163" s="28"/>
     </row>
-    <row r="164" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B164" s="9"/>
       <c r="C164" s="147"/>
       <c r="D164" s="10"/>
@@ -12504,7 +12505,7 @@
       <c r="AQ164" s="28"/>
       <c r="AR164" s="28"/>
     </row>
-    <row r="165" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B165" s="9"/>
       <c r="C165" s="147"/>
       <c r="D165" s="10"/>
@@ -12549,7 +12550,7 @@
       <c r="AQ165" s="28"/>
       <c r="AR165" s="28"/>
     </row>
-    <row r="166" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B166" s="9"/>
       <c r="C166" s="147"/>
       <c r="D166" s="10"/>
@@ -12594,7 +12595,7 @@
       <c r="AQ166" s="28"/>
       <c r="AR166" s="28"/>
     </row>
-    <row r="167" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B167" s="9"/>
       <c r="C167" s="147"/>
       <c r="D167" s="10"/>
@@ -12639,7 +12640,7 @@
       <c r="AQ167" s="28"/>
       <c r="AR167" s="28"/>
     </row>
-    <row r="168" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="9"/>
       <c r="C168" s="147"/>
       <c r="D168" s="10"/>
@@ -12684,7 +12685,7 @@
       <c r="AQ168" s="28"/>
       <c r="AR168" s="28"/>
     </row>
-    <row r="169" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B169" s="9"/>
       <c r="C169" s="147"/>
       <c r="D169" s="10"/>
@@ -12729,7 +12730,7 @@
       <c r="AQ169" s="28"/>
       <c r="AR169" s="28"/>
     </row>
-    <row r="170" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B170" s="9"/>
       <c r="C170" s="147"/>
       <c r="D170" s="10"/>
@@ -12774,7 +12775,7 @@
       <c r="AQ170" s="28"/>
       <c r="AR170" s="28"/>
     </row>
-    <row r="171" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B171" s="9"/>
       <c r="C171" s="147"/>
       <c r="D171" s="10"/>
@@ -12819,7 +12820,7 @@
       <c r="AQ171" s="28"/>
       <c r="AR171" s="28"/>
     </row>
-    <row r="172" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B172" s="9"/>
       <c r="C172" s="147"/>
       <c r="D172" s="10"/>
@@ -12864,7 +12865,7 @@
       <c r="AQ172" s="28"/>
       <c r="AR172" s="28"/>
     </row>
-    <row r="173" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B173" s="9"/>
       <c r="C173" s="147"/>
       <c r="D173" s="10"/>
@@ -12909,7 +12910,7 @@
       <c r="AQ173" s="28"/>
       <c r="AR173" s="28"/>
     </row>
-    <row r="174" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B174" s="9"/>
       <c r="C174" s="147"/>
       <c r="D174" s="10"/>
@@ -12954,7 +12955,7 @@
       <c r="AQ174" s="28"/>
       <c r="AR174" s="28"/>
     </row>
-    <row r="175" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B175" s="9"/>
       <c r="C175" s="147"/>
       <c r="D175" s="10"/>
@@ -12999,7 +13000,7 @@
       <c r="AQ175" s="28"/>
       <c r="AR175" s="28"/>
     </row>
-    <row r="176" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B176" s="9"/>
       <c r="C176" s="147"/>
       <c r="D176" s="10"/>
@@ -13044,7 +13045,7 @@
       <c r="AQ176" s="178"/>
       <c r="AR176" s="178"/>
     </row>
-    <row r="177" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B177" s="9"/>
       <c r="C177" s="147"/>
       <c r="D177" s="10"/>
@@ -13089,7 +13090,7 @@
       <c r="AQ177" s="28"/>
       <c r="AR177" s="28"/>
     </row>
-    <row r="178" spans="2:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="9"/>
       <c r="C178" s="147"/>
       <c r="D178" s="10"/>
@@ -13135,7 +13136,13 @@
       <c r="AR178" s="28"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:AR178" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B5:AR178" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="H82:I145 H148:I178 M82:N178 R82:S178 W82:X178 AB82:AC178 AG82:AH178 AL82:AM122 AM123:AN142 AM144:AN178">
     <cfRule type="expression" dxfId="47" priority="83">
       <formula>AND(G82="S",H82="")</formula>

</xml_diff>